<commit_message>
Add comprehensive project files including reviewer response strategy, analysis results, and manuscript drafts
</commit_message>
<xml_diff>
--- a/20250715_Analysis & Results/20250715_Comprehensive_Manuscript_Tables.xlsx
+++ b/20250715_Analysis & Results/20250715_Comprehensive_Manuscript_Tables.xlsx
@@ -387,7 +387,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>51</t>
+          <t>49</t>
         </is>
       </c>
     </row>
@@ -17361,7 +17361,7 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:S2"/>
+  <dimension ref="A1:T2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -17370,95 +17370,100 @@
     <row r="1" s="1" customFormat="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
+          <t>N_observations</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
           <t>N_studies</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>N_countries</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>N_journals</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>Mean_unit_size</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>Median_unit_size</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>SD_unit_size</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>Min_unit_size</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>Max_unit_size</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>Q1_unit_size</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>Q3_unit_size</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>IQR_unit_size</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>Skewness</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>Kurtosis</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>Year_range_start</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>Year_range_end</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
+      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>Temporal_span</t>
         </is>
       </c>
-      <c r="Q1" s="1" t="inlineStr">
+      <c r="R1" s="1" t="inlineStr">
         <is>
           <t>Percent_with_justification</t>
         </is>
       </c>
-      <c r="R1" s="1" t="inlineStr">
+      <c r="S1" s="1" t="inlineStr">
         <is>
           <t>Mean_total_variables</t>
         </is>
       </c>
-      <c r="S1" s="1" t="inlineStr">
+      <c r="T1" s="1" t="inlineStr">
         <is>
           <t>Median_total_variables</t>
         </is>
@@ -17469,57 +17474,60 @@
         <v>51</v>
       </c>
       <c r="B2">
+        <v>49</v>
+      </c>
+      <c r="C2">
         <v>9</v>
       </c>
-      <c r="C2">
+      <c r="D2">
         <v>27</v>
       </c>
-      <c r="D2">
+      <c r="E2">
         <v>1.63293</v>
       </c>
-      <c r="E2">
+      <c r="F2">
         <v>1.2</v>
       </c>
-      <c r="F2">
+      <c r="G2">
         <v>1.91072</v>
       </c>
-      <c r="G2">
+      <c r="H2">
         <v>0.000136</v>
       </c>
-      <c r="H2">
+      <c r="I2">
         <v>8.48</v>
       </c>
-      <c r="I2">
+      <c r="J2">
         <v>0.265</v>
       </c>
-      <c r="J2">
+      <c r="K2">
         <v>2.63</v>
       </c>
-      <c r="K2">
+      <c r="L2">
         <v>2.365</v>
       </c>
-      <c r="L2">
+      <c r="M2">
         <v>2.108</v>
       </c>
-      <c r="M2">
+      <c r="N2">
         <v>7.929</v>
       </c>
-      <c r="N2">
+      <c r="O2">
         <v>2003</v>
       </c>
-      <c r="O2">
+      <c r="P2">
         <v>2025</v>
       </c>
-      <c r="P2">
+      <c r="Q2">
         <v>22</v>
       </c>
-      <c r="Q2">
+      <c r="R2">
         <v>94.09999999999999</v>
       </c>
-      <c r="R2">
+      <c r="S2">
         <v>21.9</v>
       </c>
-      <c r="S2">
+      <c r="T2">
         <v>21</v>
       </c>
     </row>

</xml_diff>